<commit_message>
state of the art lit rev paper
</commit_message>
<xml_diff>
--- a/latex/others/literature_review.xlsx
+++ b/latex/others/literature_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b73f4100931222f3/WU/Semester 4/Thesis/git-miner/latex/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{EA5CB3BC-AE12-4F92-B732-5B58F4D40C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{61D1F3AD-DB38-4ADA-8F02-8E4BC2086A80}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{EA5CB3BC-AE12-4F92-B732-5B58F4D40C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9886A934-3D2C-4CE3-981D-FDB72CC8C689}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{D97A0909-0CE2-49C1-8DFB-44BF382C0F3D}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="370">
   <si>
     <t>Authors</t>
   </si>
@@ -1146,6 +1146,21 @@
   </si>
   <si>
     <t>Becoming a core member is mainly dependent on technical commitment (code edits) rather than reviews and commenting. A drop in certain collaborative activity predicts who will leave the core.</t>
+  </si>
+  <si>
+    <t>3 categories of research papers: structure, lifecycle and communication</t>
+  </si>
+  <si>
+    <t>Papers analyzing FLOSS lifecycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systematic literature review of OSS SNA </t>
+  </si>
+  <si>
+    <t>3 categories identified, with several subcategories each.
+Structure: core-periphery exists in a healthy OSS project, existence of core-periphery is well established
+Lifecycle: generally project leadership does not change over time, less hierarchial and more distributed over time
+temporal models are suggested as future research into project success</t>
   </si>
 </sst>
 </file>
@@ -7048,8 +7063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2E49B8-6A02-40CE-91F5-6C8877BFF8B3}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7376,6 +7391,21 @@
       </c>
       <c r="C13" s="3">
         <v>2021</v>
+      </c>
+      <c r="D13" t="s">
+        <v>366</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="H13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>